<commit_message>
Updated alarm and I/O
</commit_message>
<xml_diff>
--- a/Documentation/Software/Alarm_Logic.xlsx
+++ b/Documentation/Software/Alarm_Logic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>High Pressure Alarm</t>
   </si>
@@ -207,6 +207,9 @@
     <t>Disconnect Alarm</t>
   </si>
   <si>
+    <t>High Temperature Alarm</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -215,7 +218,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Low Pressure Alarm</t>
+      <t>Motor controller temperature</t>
     </r>
     <r>
       <rPr>
@@ -225,11 +228,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> is triggered</t>
-    </r>
-  </si>
-  <si>
-    <t>High Temperature Alarm</t>
+      <t xml:space="preserve"> is above the set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>high temperature limit</t>
+    </r>
+  </si>
+  <si>
+    <t>Apnea Alarm</t>
   </si>
   <si>
     <r>
@@ -240,7 +253,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Motor controller temperature</t>
+      <t>AC inhale wait time</t>
     </r>
     <r>
       <rPr>
@@ -250,7 +263,48 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> is above the set </t>
+      <t xml:space="preserve"> is above the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AC threshold time</t>
+    </r>
+  </si>
+  <si>
+    <t>Stop all motion; demand restart</t>
+  </si>
+  <si>
+    <t>Device Failure Alarm</t>
+  </si>
+  <si>
+    <t>Indefinite</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Motor position</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> no responding to </t>
     </r>
     <r>
       <rPr>
@@ -260,11 +314,46 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>high temperature limit</t>
-    </r>
-  </si>
-  <si>
-    <t>Apnea Alarm</t>
+      <t xml:space="preserve">commanded position </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Watchdog timeout</t>
+    </r>
+  </si>
+  <si>
+    <t>What Alarm</t>
+  </si>
+  <si>
+    <t>When Does it Occur?</t>
+  </si>
+  <si>
+    <t>What Action Does the Software Take?</t>
+  </si>
+  <si>
+    <t>How Long does the Alarm Last?</t>
+  </si>
+  <si>
+    <t>Demand device is restarted</t>
+  </si>
+  <si>
+    <t>Audible/visual alarm; stop ventilation cycle and reset to try again</t>
   </si>
   <si>
     <r>
@@ -275,17 +364,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>AC inhale wait time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is above the </t>
+      <t>Plateau pressure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is below the set</t>
     </r>
     <r>
       <rPr>
@@ -295,91 +383,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>AC threshold time</t>
-    </r>
-  </si>
-  <si>
-    <t>Stop all motion; demand restart</t>
-  </si>
-  <si>
-    <t>Device Failure Alarm</t>
-  </si>
-  <si>
-    <t>Indefinite</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Motor position</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> no responding to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">commanded position </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Watchdog timeout</t>
-    </r>
-  </si>
-  <si>
-    <t>What Alarm</t>
-  </si>
-  <si>
-    <t>When Does it Occur?</t>
-  </si>
-  <si>
-    <t>What Action Does the Software Take?</t>
-  </si>
-  <si>
-    <t>How Long does the Alarm Last?</t>
-  </si>
-  <si>
-    <t>Demand device is restarted</t>
+      <t xml:space="preserve"> low plateau pressure limit</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +428,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -437,9 +455,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,31 +842,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="77.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>10</v>
@@ -861,7 +880,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -925,8 +944,8 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -940,10 +959,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -957,10 +976,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -974,19 +993,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated diagrams and logic
</commit_message>
<xml_diff>
--- a/Documentation/Software/Alarm_Logic.xlsx
+++ b/Documentation/Software/Alarm_Logic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>High Pressure Alarm</t>
   </si>
@@ -83,6 +83,12 @@
     <t>High PEEP Alarm</t>
   </si>
   <si>
+    <t>Low PEEP Alarm</t>
+  </si>
+  <si>
+    <r>
+      <t>Measure</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -91,6 +97,204 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> PEEP pressure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is above the set</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> high PEEP pressure limit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Measure </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PEEP pressure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is below the set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>low PEEP pressure limit</t>
+    </r>
+  </si>
+  <si>
+    <t>Disable for 1-minute</t>
+  </si>
+  <si>
+    <t>Disconnect Alarm</t>
+  </si>
+  <si>
+    <t>High Temperature Alarm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Motor controller temperature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is above the set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>high temperature limit</t>
+    </r>
+  </si>
+  <si>
+    <t>Apnea Alarm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AC inhale wait time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is above the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AC threshold time</t>
+    </r>
+  </si>
+  <si>
+    <t>Stop all motion; demand restart</t>
+  </si>
+  <si>
+    <t>Indefinite</t>
+  </si>
+  <si>
+    <t>What Alarm</t>
+  </si>
+  <si>
+    <t>When Does it Occur?</t>
+  </si>
+  <si>
+    <t>What Action Does the Software Take?</t>
+  </si>
+  <si>
+    <t>How Long does the Alarm Last?</t>
+  </si>
+  <si>
+    <t>Demand device is restarted</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Plateau pressure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is below the set</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> low plateau pressure limit</t>
+    </r>
+  </si>
+  <si>
+    <t>Mechanism Failure Alarm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Measured pressure</t>
     </r>
     <r>
@@ -111,7 +315,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>high pressure limit</t>
+      <t>high pressure limit**</t>
     </r>
     <r>
       <rPr>
@@ -125,12 +329,9 @@
     </r>
   </si>
   <si>
-    <t>Low PEEP Alarm</t>
-  </si>
-  <si>
-    <r>
-      <t>Measure</t>
-    </r>
+    <t>Until next breath</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -139,7 +340,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> PEEP pressure</t>
+      <t>Motor position</t>
     </r>
     <r>
       <rPr>
@@ -149,32 +350,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> is above the set</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> high PEEP pressure limit</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Measure </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PEEP pressure</t>
+      <t xml:space="preserve"> not responding to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commanded position</t>
     </r>
     <r>
       <rPr>
@@ -184,207 +370,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> is below the set </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>low PEEP pressure limit</t>
-    </r>
-  </si>
-  <si>
-    <t>Once Dismissed/Silenced</t>
-  </si>
-  <si>
-    <t>Disable for 1-minute</t>
-  </si>
-  <si>
-    <t>Disconnect Alarm</t>
-  </si>
-  <si>
-    <t>High Temperature Alarm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Motor controller temperature</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is above the set </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>high temperature limit</t>
-    </r>
-  </si>
-  <si>
-    <t>Apnea Alarm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AC inhale wait time</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is above the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AC threshold time</t>
-    </r>
-  </si>
-  <si>
-    <t>Stop all motion; demand restart</t>
-  </si>
-  <si>
-    <t>Device Failure Alarm</t>
-  </si>
-  <si>
-    <t>Indefinite</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Motor position</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> no responding to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">commanded position </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Watchdog timeout</t>
-    </r>
-  </si>
-  <si>
-    <t>What Alarm</t>
-  </si>
-  <si>
-    <t>When Does it Occur?</t>
-  </si>
-  <si>
-    <t>What Action Does the Software Take?</t>
-  </si>
-  <si>
-    <t>How Long does the Alarm Last?</t>
-  </si>
-  <si>
-    <t>Demand device is restarted</t>
-  </si>
-  <si>
-    <t>Audible/visual alarm; stop ventilation cycle and reset to try again</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Plateau pressure</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is below the set</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> low plateau pressure limit</t>
-    </r>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>If Dismissed/Silenced by User</t>
+  </si>
+  <si>
+    <t>Audible/visual alarm; stop inhale; jump to exhale; reset to try inhale again</t>
   </si>
 </sst>
 </file>
@@ -435,12 +428,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -455,10 +466,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,16 +494,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>86845</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>135031</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>87406</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -498,8 +512,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13401675" y="123825"/>
-          <a:ext cx="4105275" cy="714375"/>
+          <a:off x="7258610" y="2040031"/>
+          <a:ext cx="4078381" cy="714375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -568,6 +582,82 @@
               </a:solidFill>
             </a:rPr>
             <a:t>Varible in blue = internal or hard-coded value</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1695450</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5143500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1695450" y="2047875"/>
+          <a:ext cx="5448300" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>** Note that the high pressure limit should be hard coded</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> to a maximum of 40 cm H2O</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -843,33 +933,33 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="77.42578125" customWidth="1"/>
-    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,16 +967,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -899,11 +989,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -911,101 +1001,101 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
+      <c r="D4" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>4</v>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>4</v>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>